<commit_message>
String Hashing done.  Working on Excel
</commit_message>
<xml_diff>
--- a/Data Tracking.xlsx
+++ b/Data Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Hash Map\Hash-Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C052CF49-664B-425D-9B00-C7EEF48B6EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325660CB-6521-45A0-B6D9-D18EC627453C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75DFD3E9-B11D-4487-91F3-099FFAFE7A5D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Check</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Table Size</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>Alpha</t>
   </si>
   <si>
@@ -67,6 +64,21 @@
   </si>
   <si>
     <t>Trial 3</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Better Hash/Probe</t>
+  </si>
+  <si>
+    <t>Collisions (Average) - String Key/Psuedo Random Probe</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>BetterHash/Probe</t>
   </si>
 </sst>
 </file>
@@ -191,134 +203,11 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Alpha</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.10009910802775025</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.20019821605550051</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30029732408325072</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.40039643211100101</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.50049554013875119</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.60059464816650143</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.70069375619425178</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.80079286422200202</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.90089197224975226</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.9990089197224975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.10009910802775025</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.20019821605550051</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30029732408325072</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.40039643211100101</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.50049554013875119</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.60059464816650143</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.70069375619425178</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.80079286422200202</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.90089197224975226</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.9990089197224975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2B83-48F1-BD44-3978EB00A425}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -352,52 +241,80 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$26:$C$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$27:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.10009910802775025</c:v>
+                  <c:v>0.100099108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20019821605550051</c:v>
+                  <c:v>0.199693369</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30029732408325072</c:v>
+                  <c:v>0.200198216</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40039643211100101</c:v>
+                  <c:v>0.300297324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50049554013875119</c:v>
+                  <c:v>0.399386738</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60059464816650143</c:v>
+                  <c:v>0.400396432</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70069375619425178</c:v>
+                  <c:v>0.50049554</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80079286422200202</c:v>
+                  <c:v>0.599080107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90089197224975226</c:v>
+                  <c:v>0.600594648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.9990089197224975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>0.700693756</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.798773476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.800792864</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.900891972</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.998466846</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99900892</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$27:$D$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$D$28:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.1112334801762114</c:v>
+                  <c:v>1.180771634759729</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.2503097893432467</c:v>
@@ -406,24 +323,36 @@
                   <c:v>1.4291784702549575</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.5484735326481398</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.6677685950413221</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.001984126984127</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>2.252853105675686</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.5037220843672454</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>3.3410596026490071</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
+                  <c:v>4.1804800500807229</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5.0199004975124391</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>10.090000000000003</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
+                  <c:v>509.54499999998944</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1008.9999999999789</c:v>
                 </c:pt>
               </c:numCache>
@@ -432,20 +361,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2B83-48F1-BD44-3978EB00A425}"/>
+              <c16:uniqueId val="{00000001-0440-4C17-AF13-69D6415785E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Trial 1</c:v>
+                  <c:v>Simple</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -475,79 +404,119 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$26:$C$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$27:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.10009910802775025</c:v>
+                  <c:v>0.100099108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20019821605550051</c:v>
+                  <c:v>0.199693369</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30029732408325072</c:v>
+                  <c:v>0.200198216</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40039643211100101</c:v>
+                  <c:v>0.300297324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50049554013875119</c:v>
+                  <c:v>0.399386738</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60059464816650143</c:v>
+                  <c:v>0.400396432</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70069375619425178</c:v>
+                  <c:v>0.50049554</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80079286422200202</c:v>
+                  <c:v>0.599080107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90089197224975226</c:v>
+                  <c:v>0.600594648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.9990089197224975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>0.700693756</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.798773476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.800792864</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.900891972</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.998466846</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99900892</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$E$27:$E$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$E$28:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>0.22500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.35000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7</c:v>
+                  <c:v>0.83333333333333326</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7</c:v>
+                  <c:v>0.91666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.15</c:v>
+                  <c:v>1.5499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>2.0583333333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8000000000000007</c:v>
+                  <c:v>2.5666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.55</c:v>
+                  <c:v>5.1833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>257.2</c:v>
+                  <c:v>7.9750000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.766666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>266.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,20 +524,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1615-4225-BB4E-69221F0BB57F}"/>
+              <c16:uniqueId val="{00000002-0440-4C17-AF13-69D6415785E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$2</c:f>
+              <c:f>Sheet1!$F$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Trial 2</c:v>
+                  <c:v>BetterHash/Probe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -598,79 +567,119 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$26:$C$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$27:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.10009910802775025</c:v>
+                  <c:v>0.100099108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20019821605550051</c:v>
+                  <c:v>0.199693369</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30029732408325072</c:v>
+                  <c:v>0.200198216</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40039643211100101</c:v>
+                  <c:v>0.300297324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50049554013875119</c:v>
+                  <c:v>0.399386738</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60059464816650143</c:v>
+                  <c:v>0.400396432</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70069375619425178</c:v>
+                  <c:v>0.50049554</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80079286422200202</c:v>
+                  <c:v>0.599080107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90089197224975226</c:v>
+                  <c:v>0.600594648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.9990089197224975</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>0.700693756</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.798773476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.800792864</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.900891972</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.998466846</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99900892</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$27:$F$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$F$28:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0.18333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.54999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9</c:v>
+                  <c:v>0.74166666666666659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.93333333333333324</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.98333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.25</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.15</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.25</c:v>
+                  <c:v>1.5166666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.35</c:v>
+                  <c:v>3.1333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55.15</c:v>
+                  <c:v>4.3416666666666668</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.733333333333334</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.016666666666666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>74.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,7 +687,143 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-1615-4225-BB4E-69221F0BB57F}"/>
+              <c16:uniqueId val="{00000003-0440-4C17-AF13-69D6415785E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>String</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$26:$C$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$27:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.100099108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.199693369</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.200198216</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.300297324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.399386738</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.400396432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50049554</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.599080107</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.600594648</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.700693756</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.798773476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.800792864</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.900891972</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.998466846</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99900892</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$G$27:$G$41</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$G$28:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.48333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.3833333333333329</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2833333333333341</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>264.41666666666669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0440-4C17-AF13-69D6415785E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -692,11 +837,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131596512"/>
-        <c:axId val="1862516512"/>
+        <c:axId val="327320496"/>
+        <c:axId val="330620208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131596512"/>
+        <c:axId val="327320496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,20 +884,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1862516512"/>
+        <c:crossAx val="330620208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1862516512"/>
+        <c:axId val="330620208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -801,7 +943,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131596512"/>
+        <c:crossAx val="327320496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -813,37 +955,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -929,7 +1040,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1037,11 +1148,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1052,11 +1158,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1088,9 +1189,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1448,23 +1546,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>499110</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EF4F9F6-8B6B-4009-BAC7-7569D5585055}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44DA478E-5D94-4281-B26F-4FD2598C677C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1782,19 +1880,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1FC033-46A1-4937-A165-E6AAA67ED6EE}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="12" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1808,49 +1908,56 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Z1" t="e">
+        <f>C3:C12,C19:C23</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1858,7 +1965,7 @@
         <v>101</v>
       </c>
       <c r="C3">
-        <f>B3/$A$18</f>
+        <f>B3/$N$3</f>
         <v>0.10009910802775025</v>
       </c>
       <c r="D3">
@@ -1891,8 +1998,11 @@
         <f>AVERAGE(I3:K3)</f>
         <v>0.11666666666666668</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1900,11 +2010,11 @@
         <v>202</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C12" si="0">B4/$A$18</f>
+        <f>B4/$N$3</f>
         <v>0.20019821605550051</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" si="1" xml:space="preserve"> 1/(1-(C4))</f>
+        <f t="shared" ref="D4:D12" si="0" xml:space="preserve"> 1/(1-(C4))</f>
         <v>1.2503097893432467</v>
       </c>
       <c r="E4">
@@ -1917,7 +2027,7 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H12" si="2">AVERAGE(E4:G4)</f>
+        <f t="shared" ref="H4:H12" si="1">AVERAGE(E4:G4)</f>
         <v>0.35000000000000003</v>
       </c>
       <c r="I4">
@@ -1930,11 +2040,11 @@
         <v>0.3</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L12" si="3">AVERAGE(I4:K4)</f>
+        <f t="shared" ref="L4:L12" si="2">AVERAGE(I4:K4)</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1942,11 +2052,11 @@
         <v>303</v>
       </c>
       <c r="C5">
+        <f>B5/$N$3</f>
+        <v>0.30029732408325072</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.30029732408325072</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
         <v>1.4291784702549575</v>
       </c>
       <c r="E5">
@@ -1959,7 +2069,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="I5">
@@ -1972,11 +2082,11 @@
         <v>0.75</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.54999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1984,11 +2094,11 @@
         <v>404</v>
       </c>
       <c r="C6">
+        <f>B6/$N$3</f>
+        <v>0.40039643211100101</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.40039643211100101</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
         <v>1.6677685950413221</v>
       </c>
       <c r="E6">
@@ -2001,7 +2111,7 @@
         <v>1.5</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="I6">
@@ -2014,11 +2124,11 @@
         <v>0.9</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.93333333333333324</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2026,11 +2136,11 @@
         <v>505</v>
       </c>
       <c r="C7">
+        <f>B7/$N$3</f>
+        <v>0.50049554013875119</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.50049554013875119</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
         <v>2.001984126984127</v>
       </c>
       <c r="E7">
@@ -2043,7 +2153,7 @@
         <v>1.05</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5499999999999998</v>
       </c>
       <c r="I7">
@@ -2056,11 +2166,11 @@
         <v>0.6</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.98333333333333339</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2068,11 +2178,11 @@
         <v>606</v>
       </c>
       <c r="C8">
+        <f>B8/$N$3</f>
+        <v>0.60059464816650143</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.60059464816650143</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
         <v>2.5037220843672454</v>
       </c>
       <c r="E8">
@@ -2085,7 +2195,7 @@
         <v>2.5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.5666666666666664</v>
       </c>
       <c r="I8">
@@ -2098,11 +2208,11 @@
         <v>1.7</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.5166666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2110,11 +2220,11 @@
         <v>707</v>
       </c>
       <c r="C9">
+        <f>B9/$N$3</f>
+        <v>0.70069375619425178</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.70069375619425178</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
         <v>3.3410596026490071</v>
       </c>
       <c r="E9">
@@ -2127,7 +2237,7 @@
         <v>5.45</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.1833333333333336</v>
       </c>
       <c r="I9">
@@ -2140,11 +2250,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.1333333333333329</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2152,11 +2262,11 @@
         <v>808</v>
       </c>
       <c r="C10">
+        <f>B10/$N$3</f>
+        <v>0.80079286422200202</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.80079286422200202</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
         <v>5.0199004975124391</v>
       </c>
       <c r="E10">
@@ -2169,7 +2279,7 @@
         <v>8.6</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10.766666666666667</v>
       </c>
       <c r="I10">
@@ -2182,11 +2292,11 @@
         <v>4.75</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.55</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2194,11 +2304,11 @@
         <v>909</v>
       </c>
       <c r="C11">
+        <f>B11/$N$3</f>
+        <v>0.90089197224975226</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.90089197224975226</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
         <v>10.090000000000003</v>
       </c>
       <c r="E11">
@@ -2211,7 +2321,7 @@
         <v>11.6</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24.25</v>
       </c>
       <c r="I11">
@@ -2224,11 +2334,11 @@
         <v>10.95</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11.733333333333334</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2236,11 +2346,11 @@
         <v>1008</v>
       </c>
       <c r="C12">
+        <f>B12/$N$3</f>
+        <v>0.9990089197224975</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>0.9990089197224975</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
         <v>1008.9999999999789</v>
       </c>
       <c r="E12">
@@ -2253,7 +2363,7 @@
         <v>384.6</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>266.55</v>
       </c>
       <c r="I12">
@@ -2266,25 +2376,470 @@
         <v>90.9</v>
       </c>
       <c r="L12">
+        <f t="shared" si="2"/>
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>521</v>
+      </c>
+      <c r="C19">
+        <f>B19/$N$19</f>
+        <v>0.19969336910693752</v>
+      </c>
+      <c r="D19">
+        <f xml:space="preserve"> 1/(1-(C19))</f>
+        <v>1.249521072796935</v>
+      </c>
+      <c r="E19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F19">
+        <v>0.25</v>
+      </c>
+      <c r="G19">
+        <v>0.65</v>
+      </c>
+      <c r="H19">
+        <f>AVERAGE(E19:G19)</f>
+        <v>0.48333333333333339</v>
+      </c>
+      <c r="N19">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>1042</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:C23" si="3">B20/$N$19</f>
+        <v>0.39938673821387505</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D23" si="4" xml:space="preserve"> 1/(1-(C20))</f>
+        <v>1.6649649010848755</v>
+      </c>
+      <c r="E20">
+        <v>1.7</v>
+      </c>
+      <c r="F20">
+        <v>1.85</v>
+      </c>
+      <c r="G20">
+        <v>1.35</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H23" si="5">AVERAGE(E20:G20)</f>
+        <v>1.6333333333333335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>1563</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="3"/>
+        <v>0.59908010732081263</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="4"/>
+        <v>2.4942638623326965</v>
+      </c>
+      <c r="E21">
+        <v>5.55</v>
+      </c>
+      <c r="F21">
+        <v>3.3</v>
+      </c>
+      <c r="G21">
+        <v>4.3</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>4.3833333333333329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>2084</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>0.7987734764277501</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="4"/>
+        <v>4.9695238095238095</v>
+      </c>
+      <c r="E22">
+        <v>6.75</v>
+      </c>
+      <c r="F22">
+        <v>7.5</v>
+      </c>
+      <c r="G22">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="5"/>
+        <v>6.2833333333333341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>2605</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>0.99846684553468767</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>652.25000000002342</v>
+      </c>
+      <c r="E23">
+        <v>186.05</v>
+      </c>
+      <c r="F23">
+        <v>374.4</v>
+      </c>
+      <c r="G23">
+        <v>232.8</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="5"/>
+        <v>264.41666666666669</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>0.10009910802775025</v>
+      </c>
+      <c r="D27">
+        <v>1.1112334801762114</v>
+      </c>
+      <c r="E27">
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="F27">
+        <v>0.11666666666666668</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>0.19969336910693752</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE(D29,D27)</f>
+        <v>1.180771634759729</v>
+      </c>
+      <c r="E28">
+        <f>AVERAGE(E29,E27)</f>
+        <v>0.22500000000000003</v>
+      </c>
+      <c r="F28">
+        <f>AVERAGE(F29,F27)</f>
+        <v>0.18333333333333335</v>
+      </c>
+      <c r="G28">
+        <v>0.48333333333333339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0.20019821605550051</v>
+      </c>
+      <c r="D29">
+        <v>1.2503097893432467</v>
+      </c>
+      <c r="E29">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="F29">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0.30029732408325072</v>
+      </c>
+      <c r="D30">
+        <v>1.4291784702549575</v>
+      </c>
+      <c r="E30">
+        <v>0.75</v>
+      </c>
+      <c r="F30">
+        <v>0.54999999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0.39938673821387505</v>
+      </c>
+      <c r="D31">
+        <f>AVERAGE(D32,D30)</f>
+        <v>1.5484735326481398</v>
+      </c>
+      <c r="E31">
+        <f>AVERAGE(E32,E30)</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="F31">
+        <f>AVERAGE(F32,F30)</f>
+        <v>0.74166666666666659</v>
+      </c>
+      <c r="G31">
+        <v>1.6333333333333335</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0.40039643211100101</v>
+      </c>
+      <c r="D32">
+        <v>1.6677685950413221</v>
+      </c>
+      <c r="E32">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F32">
+        <v>0.93333333333333324</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0.50049554013875119</v>
+      </c>
+      <c r="D33">
+        <v>2.001984126984127</v>
+      </c>
+      <c r="E33">
+        <v>1.5499999999999998</v>
+      </c>
+      <c r="F33">
+        <v>0.98333333333333339</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>0.59908010732081263</v>
+      </c>
+      <c r="D34">
+        <f>AVERAGE(D35,D33)</f>
+        <v>2.252853105675686</v>
+      </c>
+      <c r="E34">
+        <f>AVERAGE(E35,E33)</f>
+        <v>2.0583333333333331</v>
+      </c>
+      <c r="F34">
+        <f>AVERAGE(F35,F33)</f>
+        <v>1.25</v>
+      </c>
+      <c r="G34">
+        <v>4.3833333333333329</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>0.60059464816650143</v>
+      </c>
+      <c r="D35">
+        <v>2.5037220843672454</v>
+      </c>
+      <c r="E35">
+        <v>2.5666666666666664</v>
+      </c>
+      <c r="F35">
+        <v>1.5166666666666666</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>0.70069375619425178</v>
+      </c>
+      <c r="D36">
+        <v>3.3410596026490071</v>
+      </c>
+      <c r="E36">
+        <v>5.1833333333333336</v>
+      </c>
+      <c r="F36">
+        <v>3.1333333333333329</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>0.7987734764277501</v>
+      </c>
+      <c r="D37">
+        <f>AVERAGE(D38,D36)</f>
+        <v>4.1804800500807229</v>
+      </c>
+      <c r="E37">
+        <f>AVERAGE(E38,E36)</f>
+        <v>7.9750000000000005</v>
+      </c>
+      <c r="F37">
+        <f>AVERAGE(F38,F36)</f>
+        <v>4.3416666666666668</v>
+      </c>
+      <c r="G37">
+        <v>6.2833333333333341</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0.80079286422200202</v>
+      </c>
+      <c r="D38">
+        <v>5.0199004975124391</v>
+      </c>
+      <c r="E38">
+        <v>10.766666666666667</v>
+      </c>
+      <c r="F38">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0.90089197224975226</v>
+      </c>
+      <c r="D39">
+        <v>10.090000000000003</v>
+      </c>
+      <c r="E39">
+        <v>24.25</v>
+      </c>
+      <c r="F39">
+        <v>11.733333333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0.99846684553468767</v>
+      </c>
+      <c r="D40">
+        <f>AVERAGE(D41,D39)</f>
+        <v>509.54499999998944</v>
+      </c>
+      <c r="E40">
+        <f>AVERAGE(E41,E39)</f>
+        <v>145.4</v>
+      </c>
+      <c r="F40">
+        <f>AVERAGE(F41,F39)</f>
+        <v>43.016666666666666</v>
+      </c>
+      <c r="G40">
+        <v>264.41666666666669</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>0.9990089197224975</v>
+      </c>
+      <c r="D41">
+        <v>1008.9999999999789</v>
+      </c>
+      <c r="E41">
+        <v>266.55</v>
+      </c>
+      <c r="F41">
         <v>74.3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1009</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C27:G41">
+    <sortCondition ref="C27:C41"/>
+  </sortState>
+  <dataConsolidate/>
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:L1"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="E17:H17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>